<commit_message>
dades poblacio 25 amb millor config
</commit_message>
<xml_diff>
--- a/TR/PYTHON/IA2.xlsx
+++ b/TR/PYTHON/IA2.xlsx
@@ -7,6 +7,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="P-100_I-0_M-0" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="P-25_I-0_M-0" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1401,4 +1403,2042 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B125"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" t="n">
+        <v>136084.81</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>123564.68</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>149773.13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>154048.03</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>161769.43</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>156362.38</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>160706.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>164096.1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>164091.89</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>164175.92</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>19</v>
+      </c>
+      <c r="B19" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>20</v>
+      </c>
+      <c r="B20" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>21</v>
+      </c>
+      <c r="B21" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>22</v>
+      </c>
+      <c r="B22" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>23</v>
+      </c>
+      <c r="B23" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>24</v>
+      </c>
+      <c r="B24" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>25</v>
+      </c>
+      <c r="B25" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>26</v>
+      </c>
+      <c r="B26" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>27</v>
+      </c>
+      <c r="B27" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>28</v>
+      </c>
+      <c r="B28" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>29</v>
+      </c>
+      <c r="B29" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>30</v>
+      </c>
+      <c r="B30" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>31</v>
+      </c>
+      <c r="B31" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32</v>
+      </c>
+      <c r="B32" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>33</v>
+      </c>
+      <c r="B33" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>34</v>
+      </c>
+      <c r="B34" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>35</v>
+      </c>
+      <c r="B35" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>36</v>
+      </c>
+      <c r="B36" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>37</v>
+      </c>
+      <c r="B37" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>38</v>
+      </c>
+      <c r="B38" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>39</v>
+      </c>
+      <c r="B39" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>40</v>
+      </c>
+      <c r="B40" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>41</v>
+      </c>
+      <c r="B41" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>42</v>
+      </c>
+      <c r="B42" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>43</v>
+      </c>
+      <c r="B43" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>44</v>
+      </c>
+      <c r="B44" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>45</v>
+      </c>
+      <c r="B45" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>46</v>
+      </c>
+      <c r="B46" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>47</v>
+      </c>
+      <c r="B47" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>48</v>
+      </c>
+      <c r="B48" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>49</v>
+      </c>
+      <c r="B49" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>50</v>
+      </c>
+      <c r="B50" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>51</v>
+      </c>
+      <c r="B51" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>52</v>
+      </c>
+      <c r="B52" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>53</v>
+      </c>
+      <c r="B53" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>54</v>
+      </c>
+      <c r="B54" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>55</v>
+      </c>
+      <c r="B55" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>56</v>
+      </c>
+      <c r="B56" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>57</v>
+      </c>
+      <c r="B57" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>58</v>
+      </c>
+      <c r="B58" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>59</v>
+      </c>
+      <c r="B59" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>60</v>
+      </c>
+      <c r="B60" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>61</v>
+      </c>
+      <c r="B61" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>62</v>
+      </c>
+      <c r="B62" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>63</v>
+      </c>
+      <c r="B63" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>64</v>
+      </c>
+      <c r="B64" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>65</v>
+      </c>
+      <c r="B65" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>66</v>
+      </c>
+      <c r="B66" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>67</v>
+      </c>
+      <c r="B67" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>68</v>
+      </c>
+      <c r="B68" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>69</v>
+      </c>
+      <c r="B69" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>70</v>
+      </c>
+      <c r="B70" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>71</v>
+      </c>
+      <c r="B71" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>72</v>
+      </c>
+      <c r="B72" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>73</v>
+      </c>
+      <c r="B73" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>74</v>
+      </c>
+      <c r="B74" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>75</v>
+      </c>
+      <c r="B75" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>76</v>
+      </c>
+      <c r="B76" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>77</v>
+      </c>
+      <c r="B77" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>78</v>
+      </c>
+      <c r="B78" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>79</v>
+      </c>
+      <c r="B79" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>80</v>
+      </c>
+      <c r="B80" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>81</v>
+      </c>
+      <c r="B81" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>82</v>
+      </c>
+      <c r="B82" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>83</v>
+      </c>
+      <c r="B83" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>84</v>
+      </c>
+      <c r="B84" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>85</v>
+      </c>
+      <c r="B85" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>86</v>
+      </c>
+      <c r="B86" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>87</v>
+      </c>
+      <c r="B87" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>88</v>
+      </c>
+      <c r="B88" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>89</v>
+      </c>
+      <c r="B89" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>90</v>
+      </c>
+      <c r="B90" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>91</v>
+      </c>
+      <c r="B91" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>92</v>
+      </c>
+      <c r="B92" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>93</v>
+      </c>
+      <c r="B93" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>94</v>
+      </c>
+      <c r="B94" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>95</v>
+      </c>
+      <c r="B95" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>96</v>
+      </c>
+      <c r="B96" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>97</v>
+      </c>
+      <c r="B97" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>98</v>
+      </c>
+      <c r="B98" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>99</v>
+      </c>
+      <c r="B99" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>100</v>
+      </c>
+      <c r="B100" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>101</v>
+      </c>
+      <c r="B101" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>102</v>
+      </c>
+      <c r="B102" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>103</v>
+      </c>
+      <c r="B103" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>104</v>
+      </c>
+      <c r="B104" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>105</v>
+      </c>
+      <c r="B105" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>106</v>
+      </c>
+      <c r="B106" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>107</v>
+      </c>
+      <c r="B107" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>108</v>
+      </c>
+      <c r="B108" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>109</v>
+      </c>
+      <c r="B109" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>110</v>
+      </c>
+      <c r="B110" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>111</v>
+      </c>
+      <c r="B111" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>112</v>
+      </c>
+      <c r="B112" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>113</v>
+      </c>
+      <c r="B113" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>114</v>
+      </c>
+      <c r="B114" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>115</v>
+      </c>
+      <c r="B115" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>116</v>
+      </c>
+      <c r="B116" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>117</v>
+      </c>
+      <c r="B117" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>118</v>
+      </c>
+      <c r="B118" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>119</v>
+      </c>
+      <c r="B119" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>120</v>
+      </c>
+      <c r="B120" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>121</v>
+      </c>
+      <c r="B121" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>122</v>
+      </c>
+      <c r="B122" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>123</v>
+      </c>
+      <c r="B123" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>124</v>
+      </c>
+      <c r="B124" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>125</v>
+      </c>
+      <c r="B125" t="n">
+        <v>164188.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B125"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" t="n">
+        <v>60746.02</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>97582.13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>106292.72</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>127835.4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>138523.04</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>140797.61</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>137955.1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>149605.42</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>144698.25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>146372.64</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>140223.55</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>163758.43</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>158055.62</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>153427.12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" t="n">
+        <v>156236.33</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" t="n">
+        <v>160520.78</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" t="n">
+        <v>159708.48</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" t="n">
+        <v>161423.93</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>19</v>
+      </c>
+      <c r="B19" t="n">
+        <v>163917.35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>20</v>
+      </c>
+      <c r="B20" t="n">
+        <v>163939.38</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>21</v>
+      </c>
+      <c r="B21" t="n">
+        <v>161032.07</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>22</v>
+      </c>
+      <c r="B22" t="n">
+        <v>163976.92</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>23</v>
+      </c>
+      <c r="B23" t="n">
+        <v>163963.69</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>24</v>
+      </c>
+      <c r="B24" t="n">
+        <v>163977.95</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>25</v>
+      </c>
+      <c r="B25" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>26</v>
+      </c>
+      <c r="B26" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>27</v>
+      </c>
+      <c r="B27" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>28</v>
+      </c>
+      <c r="B28" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>29</v>
+      </c>
+      <c r="B29" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>30</v>
+      </c>
+      <c r="B30" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>31</v>
+      </c>
+      <c r="B31" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32</v>
+      </c>
+      <c r="B32" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>33</v>
+      </c>
+      <c r="B33" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>34</v>
+      </c>
+      <c r="B34" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>35</v>
+      </c>
+      <c r="B35" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>36</v>
+      </c>
+      <c r="B36" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>37</v>
+      </c>
+      <c r="B37" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>38</v>
+      </c>
+      <c r="B38" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>39</v>
+      </c>
+      <c r="B39" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>40</v>
+      </c>
+      <c r="B40" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>41</v>
+      </c>
+      <c r="B41" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>42</v>
+      </c>
+      <c r="B42" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>43</v>
+      </c>
+      <c r="B43" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>44</v>
+      </c>
+      <c r="B44" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>45</v>
+      </c>
+      <c r="B45" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>46</v>
+      </c>
+      <c r="B46" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>47</v>
+      </c>
+      <c r="B47" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>48</v>
+      </c>
+      <c r="B48" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>49</v>
+      </c>
+      <c r="B49" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>50</v>
+      </c>
+      <c r="B50" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>51</v>
+      </c>
+      <c r="B51" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>52</v>
+      </c>
+      <c r="B52" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>53</v>
+      </c>
+      <c r="B53" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>54</v>
+      </c>
+      <c r="B54" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>55</v>
+      </c>
+      <c r="B55" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>56</v>
+      </c>
+      <c r="B56" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>57</v>
+      </c>
+      <c r="B57" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>58</v>
+      </c>
+      <c r="B58" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>59</v>
+      </c>
+      <c r="B59" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>60</v>
+      </c>
+      <c r="B60" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>61</v>
+      </c>
+      <c r="B61" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>62</v>
+      </c>
+      <c r="B62" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>63</v>
+      </c>
+      <c r="B63" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>64</v>
+      </c>
+      <c r="B64" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>65</v>
+      </c>
+      <c r="B65" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>66</v>
+      </c>
+      <c r="B66" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>67</v>
+      </c>
+      <c r="B67" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>68</v>
+      </c>
+      <c r="B68" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>69</v>
+      </c>
+      <c r="B69" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>70</v>
+      </c>
+      <c r="B70" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>71</v>
+      </c>
+      <c r="B71" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>72</v>
+      </c>
+      <c r="B72" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>73</v>
+      </c>
+      <c r="B73" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>74</v>
+      </c>
+      <c r="B74" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>75</v>
+      </c>
+      <c r="B75" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>76</v>
+      </c>
+      <c r="B76" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>77</v>
+      </c>
+      <c r="B77" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>78</v>
+      </c>
+      <c r="B78" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>79</v>
+      </c>
+      <c r="B79" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>80</v>
+      </c>
+      <c r="B80" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>81</v>
+      </c>
+      <c r="B81" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>82</v>
+      </c>
+      <c r="B82" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>83</v>
+      </c>
+      <c r="B83" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>84</v>
+      </c>
+      <c r="B84" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>85</v>
+      </c>
+      <c r="B85" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>86</v>
+      </c>
+      <c r="B86" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>87</v>
+      </c>
+      <c r="B87" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>88</v>
+      </c>
+      <c r="B88" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>89</v>
+      </c>
+      <c r="B89" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>90</v>
+      </c>
+      <c r="B90" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>91</v>
+      </c>
+      <c r="B91" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>92</v>
+      </c>
+      <c r="B92" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>93</v>
+      </c>
+      <c r="B93" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>94</v>
+      </c>
+      <c r="B94" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>95</v>
+      </c>
+      <c r="B95" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>96</v>
+      </c>
+      <c r="B96" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>97</v>
+      </c>
+      <c r="B97" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>98</v>
+      </c>
+      <c r="B98" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>99</v>
+      </c>
+      <c r="B99" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>100</v>
+      </c>
+      <c r="B100" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>101</v>
+      </c>
+      <c r="B101" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>102</v>
+      </c>
+      <c r="B102" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>103</v>
+      </c>
+      <c r="B103" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>104</v>
+      </c>
+      <c r="B104" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>105</v>
+      </c>
+      <c r="B105" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>106</v>
+      </c>
+      <c r="B106" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>107</v>
+      </c>
+      <c r="B107" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>108</v>
+      </c>
+      <c r="B108" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>109</v>
+      </c>
+      <c r="B109" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>110</v>
+      </c>
+      <c r="B110" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>111</v>
+      </c>
+      <c r="B111" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>112</v>
+      </c>
+      <c r="B112" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>113</v>
+      </c>
+      <c r="B113" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>114</v>
+      </c>
+      <c r="B114" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>115</v>
+      </c>
+      <c r="B115" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>116</v>
+      </c>
+      <c r="B116" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>117</v>
+      </c>
+      <c r="B117" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>118</v>
+      </c>
+      <c r="B118" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>119</v>
+      </c>
+      <c r="B119" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>120</v>
+      </c>
+      <c r="B120" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>121</v>
+      </c>
+      <c r="B121" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>122</v>
+      </c>
+      <c r="B122" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>123</v>
+      </c>
+      <c r="B123" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>124</v>
+      </c>
+      <c r="B124" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>125</v>
+      </c>
+      <c r="B125" t="n">
+        <v>163998.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>